<commit_message>
capability to ignore artists, better deleted events handling and other stuff
</commit_message>
<xml_diff>
--- a/resources/country_cleaning.xlsx
+++ b/resources/country_cleaning.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>clean</t>
   </si>
@@ -176,6 +176,15 @@
   </si>
   <si>
     <t>Palestine</t>
+  </si>
+  <si>
+    <t>LUX</t>
+  </si>
+  <si>
+    <t>Luxemburg</t>
+  </si>
+  <si>
+    <t>Democratic Republic of the Congo</t>
   </si>
 </sst>
 </file>
@@ -524,7 +533,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -859,6 +868,28 @@
         <v>53</v>
       </c>
     </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
delete files that do not belong in repo
</commit_message>
<xml_diff>
--- a/resources/country_cleaning.xlsx
+++ b/resources/country_cleaning.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\git\buitenlandse_concerten_grabber\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>clean</t>
   </si>
@@ -178,35 +183,39 @@
     <t>Palestine</t>
   </si>
   <si>
-    <t>LUX</t>
+    <t>LU</t>
   </si>
   <si>
     <t>Luxemburg</t>
   </si>
   <si>
     <t>Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>nan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -221,26 +230,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -528,20 +554,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,8 +571,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -560,8 +582,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -571,8 +593,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -582,8 +604,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -593,8 +615,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -604,8 +626,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -615,8 +637,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -626,8 +648,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -637,8 +659,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -648,8 +670,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -659,8 +681,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -670,8 +692,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -681,8 +703,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -692,8 +714,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -703,8 +725,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -714,8 +736,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -725,8 +747,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -736,8 +758,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -747,8 +769,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -758,8 +780,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -769,8 +791,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -780,8 +802,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -791,8 +813,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -802,8 +824,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -813,8 +835,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -824,8 +846,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -835,8 +857,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -846,8 +868,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1" t="n">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
@@ -857,8 +879,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1" t="n">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
@@ -868,8 +890,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1" t="n">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
@@ -879,8 +901,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1" t="n">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -890,7 +912,18 @@
         <v>56</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>